<commit_message>
Fixed missing references to LocalizedTexts and continue to implement ProvenanceNFTItem
</commit_message>
<xml_diff>
--- a/Localization/Texts.xlsx
+++ b/Localization/Texts.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UnitySSD\VoxToVFX\Localization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UnitySSD\VoxToVFX-2021\Localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A062A920-DD2C-4948-B564-6B313EF8F364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA1908C-B705-48A9-85CC-FB724BD46DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2318,13 +2318,13 @@
     <t>[BUY_NOW_REMOVED_LABEL]</t>
   </si>
   <si>
-    <t>Transfered from {0} to {1}</t>
-  </si>
-  <si>
     <t>Transféré par {0} à {1}</t>
   </si>
   <si>
-    <t>[TRANSFERD_FROM_TO_LABEL]</t>
+    <t>[TRANSFERRED_FROM_TO_LABEL]</t>
+  </si>
+  <si>
+    <t>Transferred from {0} to {1}</t>
   </si>
 </sst>
 </file>
@@ -2784,7 +2784,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A242" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A260" sqref="A260"/>
+      <selection pane="bottomLeft" activeCell="E262" sqref="E262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6037,13 +6037,13 @@
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="D259" s="2" t="s">
+        <v>754</v>
+      </c>
+      <c r="E259" s="2" t="s">
         <v>756</v>
-      </c>
-      <c r="D259" s="2" t="s">
-        <v>755</v>
-      </c>
-      <c r="E259" s="2" t="s">
-        <v>754</v>
       </c>
     </row>
   </sheetData>
@@ -6055,6 +6055,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="88b2ba63-7ebb-4a2a-9e9c-c27acabcde36">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="6bab19be-6345-4ed3-a392-384eca2a3a3f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005460182F725DE045861B6A88650F6BEB" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="d6f2dc6f3d7fbcfe24006b02fd61b3cf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="88b2ba63-7ebb-4a2a-9e9c-c27acabcde36" xmlns:ns3="6bab19be-6345-4ed3-a392-384eca2a3a3f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1cf88c42ef435e36ebab6d4c7e4dc2e7" ns2:_="" ns3:_="">
     <xsd:import namespace="88b2ba63-7ebb-4a2a-9e9c-c27acabcde36"/>
@@ -6297,17 +6308,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="88b2ba63-7ebb-4a2a-9e9c-c27acabcde36">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="6bab19be-6345-4ed3-a392-384eca2a3a3f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -6318,6 +6318,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7732749D-B1A2-4E70-B7F4-898D2C27DFCA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="88b2ba63-7ebb-4a2a-9e9c-c27acabcde36"/>
+    <ds:schemaRef ds:uri="6bab19be-6345-4ed3-a392-384eca2a3a3f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5151E3F2-6D7E-4401-BC66-ED7AF20F0E43}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6336,17 +6347,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7732749D-B1A2-4E70-B7F4-898D2C27DFCA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="88b2ba63-7ebb-4a2a-9e9c-c27acabcde36"/>
-    <ds:schemaRef ds:uri="6bab19be-6345-4ed3-a392-384eca2a3a3f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4394CFF6-4A26-4CEA-BFC4-481182046E8E}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Split the NFTUpdatePanel into small components
</commit_message>
<xml_diff>
--- a/Localization/Texts.xlsx
+++ b/Localization/Texts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UnitySSD\VoxToVFX-2021\Localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA1908C-B705-48A9-85CC-FB724BD46DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEEE49FD-C0B9-423D-A564-27682872396D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="757">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="783">
   <si>
     <t>Clé</t>
   </si>
@@ -2325,6 +2325,84 @@
   </si>
   <si>
     <t>Transferred from {0} to {1}</t>
+  </si>
+  <si>
+    <t>[BUY_NOW_TITLE]</t>
+  </si>
+  <si>
+    <t>[BUY_NOW_DESCRIPTION]</t>
+  </si>
+  <si>
+    <t>Once the transaction is confirmed, the NFT will be sent to your wallet instantly.</t>
+  </si>
+  <si>
+    <t>Une fois la transaction confirmée, le NFT sera envoyé instantanément à votre portefeuille.</t>
+  </si>
+  <si>
+    <t>Available Balance</t>
+  </si>
+  <si>
+    <t>Balance disponible</t>
+  </si>
+  <si>
+    <t>[AVAILABLE_BALANCE_LABEL]</t>
+  </si>
+  <si>
+    <t>Marketplace Balance</t>
+  </si>
+  <si>
+    <t>Wallet Balance</t>
+  </si>
+  <si>
+    <t>[MARKETPLACE_BALANCE_LABEL]</t>
+  </si>
+  <si>
+    <t>[WALLET_BALANCE_LABEL]</t>
+  </si>
+  <si>
+    <t>You do not have enough ETH</t>
+  </si>
+  <si>
+    <t>Vous n'avez pas assez d'ETH</t>
+  </si>
+  <si>
+    <t>[BUY_NOW_NOT_ENOUGH_ETH]</t>
+  </si>
+  <si>
+    <t>Buying …</t>
+  </si>
+  <si>
+    <t>En cours d'achat …</t>
+  </si>
+  <si>
+    <t>[BUY_NOW_WAITING_TITLE]</t>
+  </si>
+  <si>
+    <t>[BUY_NOW_WAITING_DESCRIPTION]</t>
+  </si>
+  <si>
+    <t>The sale is being confirmed on the Ethereum blockchain.</t>
+  </si>
+  <si>
+    <t>La vente est en cours de confirmation sur la blockchain Ethereum.</t>
+  </si>
+  <si>
+    <t>You got it !</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vous l'avez ! </t>
+  </si>
+  <si>
+    <t>[BUY_NOW_SUCCESS_TITLE]</t>
+  </si>
+  <si>
+    <t>[BUY_NOW_SUCCESS_DESCRIPTION]</t>
+  </si>
+  <si>
+    <t>You got the NFT for {0} ETH</t>
+  </si>
+  <si>
+    <t>Vous avez eu le NFT pour {0} ETH</t>
   </si>
 </sst>
 </file>
@@ -2780,11 +2858,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:IW259"/>
+  <dimension ref="A1:IW269"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A242" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E262" sqref="E262"/>
+      <pane ySplit="1" topLeftCell="A247" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D269" sqref="D269"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6044,6 +6122,116 @@
       </c>
       <c r="E259" s="2" t="s">
         <v>756</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A260" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="D260" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="E260" s="2" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A261" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="D261" s="2" t="s">
+        <v>760</v>
+      </c>
+      <c r="E261" s="2" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A262" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="D262" s="2" t="s">
+        <v>762</v>
+      </c>
+      <c r="E262" s="2" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A263" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="D263" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="E263" s="2" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A264" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="D264" s="2" t="s">
+        <v>765</v>
+      </c>
+      <c r="E264" s="2" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A265" s="1" t="s">
+        <v>770</v>
+      </c>
+      <c r="D265" s="2" t="s">
+        <v>769</v>
+      </c>
+      <c r="E265" s="2" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A266" s="1" t="s">
+        <v>773</v>
+      </c>
+      <c r="D266" s="2" t="s">
+        <v>772</v>
+      </c>
+      <c r="E266" s="2" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A267" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="D267" s="2" t="s">
+        <v>776</v>
+      </c>
+      <c r="E267" s="2" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A268" s="1" t="s">
+        <v>779</v>
+      </c>
+      <c r="D268" s="2" t="s">
+        <v>778</v>
+      </c>
+      <c r="E268" s="2" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A269" s="1" t="s">
+        <v>780</v>
+      </c>
+      <c r="D269" s="2" t="s">
+        <v>782</v>
+      </c>
+      <c r="E269" s="2" t="s">
+        <v>781</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed retry button in Confirmation wallet popup in case of error and fixed small typo error
</commit_message>
<xml_diff>
--- a/Localization/Texts.xlsx
+++ b/Localization/Texts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UnitySSD\VoxToVFX-2021\Localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEEE49FD-C0B9-423D-A564-27682872396D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B4E9A2-1772-4B56-AD05-A074CF335AAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2048,9 +2048,6 @@
     <t>Transferring …</t>
   </si>
   <si>
-    <t>[TRANSFER_NFT_WAITING_DESCRPTION]</t>
-  </si>
-  <si>
     <t>The NFT is being transferred on the Ethereum blockchain</t>
   </si>
   <si>
@@ -2403,6 +2400,9 @@
   </si>
   <si>
     <t>Vous avez eu le NFT pour {0} ETH</t>
+  </si>
+  <si>
+    <t>[TRANSFER_NFT_WAITING_DESCRIPTION]</t>
   </si>
 </sst>
 </file>
@@ -2861,8 +2861,8 @@
   <dimension ref="A1:IW269"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A247" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D269" sqref="D269"/>
+      <pane ySplit="1" topLeftCell="A200" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A217" sqref="A217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4735,10 +4735,10 @@
         <v>464</v>
       </c>
       <c r="D158" s="2" t="s">
+        <v>693</v>
+      </c>
+      <c r="E158" s="2" t="s">
         <v>694</v>
-      </c>
-      <c r="E158" s="2" t="s">
-        <v>695</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
@@ -5579,7 +5579,7 @@
         <v>603</v>
       </c>
       <c r="D210" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="E210" s="2" t="s">
         <v>604</v>
@@ -5642,35 +5642,35 @@
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="D216" s="2" t="s">
+        <v>665</v>
+      </c>
+      <c r="E216" s="2" t="s">
         <v>664</v>
-      </c>
-      <c r="D216" s="2" t="s">
-        <v>666</v>
-      </c>
-      <c r="E216" s="2" t="s">
-        <v>665</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="D217" s="2" t="s">
+        <v>668</v>
+      </c>
+      <c r="E217" s="2" t="s">
         <v>667</v>
-      </c>
-      <c r="D217" s="2" t="s">
-        <v>669</v>
-      </c>
-      <c r="E217" s="2" t="s">
-        <v>668</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="D218" s="2" t="s">
+        <v>671</v>
+      </c>
+      <c r="E218" s="2" t="s">
         <v>670</v>
-      </c>
-      <c r="D218" s="2" t="s">
-        <v>672</v>
-      </c>
-      <c r="E218" s="2" t="s">
-        <v>671</v>
       </c>
     </row>
     <row r="219" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5818,260 +5818,260 @@
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="D232" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="E232" s="2" t="s">
         <v>678</v>
-      </c>
-      <c r="E232" s="2" t="s">
-        <v>679</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="D233" s="2" t="s">
+        <v>679</v>
+      </c>
+      <c r="E233" s="2" t="s">
         <v>680</v>
-      </c>
-      <c r="E233" s="2" t="s">
-        <v>681</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="D234" s="2" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="E234" s="2" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="D235" s="2" t="s">
+        <v>683</v>
+      </c>
+      <c r="E235" s="2" t="s">
         <v>684</v>
-      </c>
-      <c r="E235" s="2" t="s">
-        <v>685</v>
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="D236" s="2" t="s">
+        <v>685</v>
+      </c>
+      <c r="E236" s="2" t="s">
         <v>686</v>
-      </c>
-      <c r="E236" s="2" t="s">
-        <v>687</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="D237" s="2" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="E237" s="2" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="D238" s="2" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="E238" s="2" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
+        <v>719</v>
+      </c>
+      <c r="D239" s="2" t="s">
         <v>720</v>
       </c>
-      <c r="D239" s="2" t="s">
+      <c r="E239" s="2" t="s">
         <v>721</v>
-      </c>
-      <c r="E239" s="2" t="s">
-        <v>722</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
+        <v>695</v>
+      </c>
+      <c r="D240" s="2" t="s">
         <v>696</v>
       </c>
-      <c r="D240" s="2" t="s">
+      <c r="E240" s="2" t="s">
         <v>697</v>
-      </c>
-      <c r="E240" s="2" t="s">
-        <v>698</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="D241" s="2" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="E241" s="2" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="242" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D242" s="2" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="E242" s="2" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D243" s="2" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="E243" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="244" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
+        <v>710</v>
+      </c>
+      <c r="D244" s="2" t="s">
         <v>711</v>
       </c>
-      <c r="D244" s="2" t="s">
-        <v>712</v>
-      </c>
       <c r="E244" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="D245" s="2" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="E245" s="2" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="246" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="D246" s="2" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="E246" s="2" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="D247" s="2" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="E247" s="2" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="D248" s="2" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="E248" s="2" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="D249" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="E249" s="2" t="s">
         <v>725</v>
-      </c>
-      <c r="D249" s="2" t="s">
-        <v>728</v>
-      </c>
-      <c r="E249" s="2" t="s">
-        <v>726</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="D250" s="2" t="s">
+        <v>731</v>
+      </c>
+      <c r="E250" s="2" t="s">
         <v>729</v>
-      </c>
-      <c r="D250" s="2" t="s">
-        <v>732</v>
-      </c>
-      <c r="E250" s="2" t="s">
-        <v>730</v>
       </c>
     </row>
     <row r="251" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="D251" s="2" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E251" s="2" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="D252" s="2" t="s">
         <v>736</v>
       </c>
-      <c r="D252" s="2" t="s">
-        <v>737</v>
-      </c>
       <c r="E252" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="D253" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="E253" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="D254" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E254" s="2" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="D255" s="2" t="s">
         <v>540</v>
@@ -6082,51 +6082,51 @@
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
+        <v>745</v>
+      </c>
+      <c r="D256" s="2" t="s">
         <v>746</v>
       </c>
-      <c r="D256" s="2" t="s">
-        <v>747</v>
-      </c>
       <c r="E256" s="2" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="D257" s="2" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E257" s="2" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="D258" s="2" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="E258" s="2" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="D259" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="E259" s="2" t="s">
         <v>755</v>
-      </c>
-      <c r="D259" s="2" t="s">
-        <v>754</v>
-      </c>
-      <c r="E259" s="2" t="s">
-        <v>756</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="D260" s="2" t="s">
         <v>497</v>
@@ -6137,101 +6137,101 @@
     </row>
     <row r="261" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="D261" s="2" t="s">
+        <v>759</v>
+      </c>
+      <c r="E261" s="2" t="s">
         <v>758</v>
-      </c>
-      <c r="D261" s="2" t="s">
-        <v>760</v>
-      </c>
-      <c r="E261" s="2" t="s">
-        <v>759</v>
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="D262" s="2" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="E262" s="2" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="D263" s="2" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="E263" s="2" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="D264" s="2" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="E264" s="2" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="D265" s="2" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="E265" s="2" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="D266" s="2" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="E266" s="2" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
+        <v>773</v>
+      </c>
+      <c r="D267" s="2" t="s">
+        <v>775</v>
+      </c>
+      <c r="E267" s="2" t="s">
         <v>774</v>
-      </c>
-      <c r="D267" s="2" t="s">
-        <v>776</v>
-      </c>
-      <c r="E267" s="2" t="s">
-        <v>775</v>
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="D268" s="2" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="E268" s="2" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
+        <v>779</v>
+      </c>
+      <c r="D269" s="2" t="s">
+        <v>781</v>
+      </c>
+      <c r="E269" s="2" t="s">
         <v>780</v>
-      </c>
-      <c r="D269" s="2" t="s">
-        <v>782</v>
-      </c>
-      <c r="E269" s="2" t="s">
-        <v>781</v>
       </c>
     </row>
   </sheetData>
@@ -6243,17 +6243,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="88b2ba63-7ebb-4a2a-9e9c-c27acabcde36">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="6bab19be-6345-4ed3-a392-384eca2a3a3f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005460182F725DE045861B6A88650F6BEB" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="d6f2dc6f3d7fbcfe24006b02fd61b3cf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="88b2ba63-7ebb-4a2a-9e9c-c27acabcde36" xmlns:ns3="6bab19be-6345-4ed3-a392-384eca2a3a3f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1cf88c42ef435e36ebab6d4c7e4dc2e7" ns2:_="" ns3:_="">
     <xsd:import namespace="88b2ba63-7ebb-4a2a-9e9c-c27acabcde36"/>
@@ -6496,6 +6485,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="88b2ba63-7ebb-4a2a-9e9c-c27acabcde36">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="6bab19be-6345-4ed3-a392-384eca2a3a3f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -6506,17 +6506,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7732749D-B1A2-4E70-B7F4-898D2C27DFCA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="88b2ba63-7ebb-4a2a-9e9c-c27acabcde36"/>
-    <ds:schemaRef ds:uri="6bab19be-6345-4ed3-a392-384eca2a3a3f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5151E3F2-6D7E-4401-BC66-ED7AF20F0E43}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6535,6 +6524,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7732749D-B1A2-4E70-B7F4-898D2C27DFCA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="88b2ba63-7ebb-4a2a-9e9c-c27acabcde36"/>
+    <ds:schemaRef ds:uri="6bab19be-6345-4ed3-a392-384eca2a3a3f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4394CFF6-4A26-4CEA-BFC4-481182046E8E}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Display a message if there is no created/collections/owned items of the profile panel
</commit_message>
<xml_diff>
--- a/Localization/Texts.xlsx
+++ b/Localization/Texts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UnitySSD\VoxToVFX-2021\Localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B4E9A2-1772-4B56-AD05-A074CF335AAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F39E01-C836-4C64-A038-910EE7DEACA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="783">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="792">
   <si>
     <t>Clé</t>
   </si>
@@ -2403,6 +2403,33 @@
   </si>
   <si>
     <t>[TRANSFER_NFT_WAITING_DESCRIPTION]</t>
+  </si>
+  <si>
+    <t>[PROFILE_NO_CREATED_ITEMS]</t>
+  </si>
+  <si>
+    <t>[PROFILE_NO_CREATED_COLLECTIONS]</t>
+  </si>
+  <si>
+    <t>[PROFILE_NO_OWNED_ITEMS]</t>
+  </si>
+  <si>
+    <t>Cet utilisateur ne possède aucun NFT sur VoxVerse</t>
+  </si>
+  <si>
+    <t>Cet utilisateur n'a pas encore créé de NFTs sur VoxVerse</t>
+  </si>
+  <si>
+    <t>Cet utilisateur n'a pas encore créé de collections sur VoxVerse</t>
+  </si>
+  <si>
+    <t>This user has not yet created any NFTs on VoxVerse</t>
+  </si>
+  <si>
+    <t>This user has not created any collections yet on VoxVerse</t>
+  </si>
+  <si>
+    <t>This user does not own any NFTs on VoxVerse</t>
   </si>
 </sst>
 </file>
@@ -2858,11 +2885,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:IW269"/>
+  <dimension ref="A1:IW272"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A200" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A217" sqref="A217"/>
+      <pane ySplit="1" topLeftCell="A247" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E275" sqref="E275"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6234,6 +6261,39 @@
         <v>780</v>
       </c>
     </row>
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A270" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="D270" s="2" t="s">
+        <v>787</v>
+      </c>
+      <c r="E270" s="2" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A271" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="D271" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="E271" s="2" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A272" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="D272" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="E272" s="2" t="s">
+        <v>791</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:IW163" xr:uid="{638B181E-C938-4D12-8294-8F02EFDDDA97}"/>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -6243,6 +6303,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="88b2ba63-7ebb-4a2a-9e9c-c27acabcde36">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="6bab19be-6345-4ed3-a392-384eca2a3a3f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005460182F725DE045861B6A88650F6BEB" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="d6f2dc6f3d7fbcfe24006b02fd61b3cf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="88b2ba63-7ebb-4a2a-9e9c-c27acabcde36" xmlns:ns3="6bab19be-6345-4ed3-a392-384eca2a3a3f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1cf88c42ef435e36ebab6d4c7e4dc2e7" ns2:_="" ns3:_="">
     <xsd:import namespace="88b2ba63-7ebb-4a2a-9e9c-c27acabcde36"/>
@@ -6485,17 +6556,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="88b2ba63-7ebb-4a2a-9e9c-c27acabcde36">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="6bab19be-6345-4ed3-a392-384eca2a3a3f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -6506,6 +6566,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7732749D-B1A2-4E70-B7F4-898D2C27DFCA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="88b2ba63-7ebb-4a2a-9e9c-c27acabcde36"/>
+    <ds:schemaRef ds:uri="6bab19be-6345-4ed3-a392-384eca2a3a3f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5151E3F2-6D7E-4401-BC66-ED7AF20F0E43}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6524,17 +6595,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7732749D-B1A2-4E70-B7F4-898D2C27DFCA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="88b2ba63-7ebb-4a2a-9e9c-c27acabcde36"/>
-    <ds:schemaRef ds:uri="6bab19be-6345-4ed3-a392-384eca2a3a3f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4394CFF6-4A26-4CEA-BFC4-481182046E8E}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Buy function is now wokring
</commit_message>
<xml_diff>
--- a/Localization/Texts.xlsx
+++ b/Localization/Texts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UnitySSD\VoxToVFX-2021\Localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F39E01-C836-4C64-A038-910EE7DEACA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63EEE9FC-0026-4246-A4A9-F6C47D4175C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Texts!$A$1:$IW$163</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="792">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="798">
   <si>
     <t>Clé</t>
   </si>
@@ -2430,6 +2431,24 @@
   </si>
   <si>
     <t>This user does not own any NFTs on VoxVerse</t>
+  </si>
+  <si>
+    <t>[CONFIRM]</t>
+  </si>
+  <si>
+    <t>Confirmer</t>
+  </si>
+  <si>
+    <t>Confirm</t>
+  </si>
+  <si>
+    <t>[BOUGHT_BY_LABEL]</t>
+  </si>
+  <si>
+    <t>Acheté par</t>
+  </si>
+  <si>
+    <t>Bought by</t>
   </si>
 </sst>
 </file>
@@ -2885,11 +2904,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:IW272"/>
+  <dimension ref="A1:IW274"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A247" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E275" sqref="E275"/>
+      <selection pane="bottomLeft" activeCell="A258" sqref="A258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6120,178 +6139,200 @@
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
-        <v>749</v>
+        <v>795</v>
       </c>
       <c r="D257" s="2" t="s">
-        <v>748</v>
+        <v>796</v>
       </c>
       <c r="E257" s="2" t="s">
-        <v>747</v>
+        <v>797</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="D258" s="2" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="E258" s="2" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="D259" s="2" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="E259" s="2" t="s">
-        <v>755</v>
+        <v>750</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="D260" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="E260" s="2" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A261" s="1" t="s">
         <v>756</v>
       </c>
-      <c r="D260" s="2" t="s">
+      <c r="D261" s="2" t="s">
         <v>497</v>
       </c>
-      <c r="E260" s="2" t="s">
+      <c r="E261" s="2" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="261" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A261" s="1" t="s">
+    <row r="262" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A262" s="1" t="s">
         <v>757</v>
       </c>
-      <c r="D261" s="2" t="s">
+      <c r="D262" s="2" t="s">
         <v>759</v>
       </c>
-      <c r="E261" s="2" t="s">
+      <c r="E262" s="2" t="s">
         <v>758</v>
-      </c>
-    </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A262" s="1" t="s">
-        <v>762</v>
-      </c>
-      <c r="D262" s="2" t="s">
-        <v>761</v>
-      </c>
-      <c r="E262" s="2" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="D263" s="2" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="E263" s="2" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="D264" s="2" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="E264" s="2" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="D265" s="2" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
       <c r="E265" s="2" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="D266" s="2" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="E266" s="2" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="D267" s="2" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="E267" s="2" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
-        <v>778</v>
+        <v>773</v>
       </c>
       <c r="D268" s="2" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="E268" s="2" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="D269" s="2" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
       <c r="E269" s="2" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="D270" s="2" t="s">
-        <v>787</v>
+        <v>781</v>
       </c>
       <c r="E270" s="2" t="s">
-        <v>789</v>
+        <v>780</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="D271" s="2" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="E271" s="2" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="D272" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="E272" s="2" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A273" s="1" t="s">
         <v>785</v>
       </c>
-      <c r="D272" s="2" t="s">
+      <c r="D273" s="2" t="s">
         <v>786</v>
       </c>
-      <c r="E272" s="2" t="s">
+      <c r="E273" s="2" t="s">
         <v>791</v>
+      </c>
+    </row>
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A274" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="D274" s="2" t="s">
+        <v>793</v>
+      </c>
+      <c r="E274" s="2" t="s">
+        <v>794</v>
       </c>
     </row>
   </sheetData>
@@ -6303,17 +6344,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="88b2ba63-7ebb-4a2a-9e9c-c27acabcde36">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="6bab19be-6345-4ed3-a392-384eca2a3a3f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005460182F725DE045861B6A88650F6BEB" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="d6f2dc6f3d7fbcfe24006b02fd61b3cf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="88b2ba63-7ebb-4a2a-9e9c-c27acabcde36" xmlns:ns3="6bab19be-6345-4ed3-a392-384eca2a3a3f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1cf88c42ef435e36ebab6d4c7e4dc2e7" ns2:_="" ns3:_="">
     <xsd:import namespace="88b2ba63-7ebb-4a2a-9e9c-c27acabcde36"/>
@@ -6556,6 +6586,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="88b2ba63-7ebb-4a2a-9e9c-c27acabcde36">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="6bab19be-6345-4ed3-a392-384eca2a3a3f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -6566,17 +6607,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7732749D-B1A2-4E70-B7F4-898D2C27DFCA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="88b2ba63-7ebb-4a2a-9e9c-c27acabcde36"/>
-    <ds:schemaRef ds:uri="6bab19be-6345-4ed3-a392-384eca2a3a3f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5151E3F2-6D7E-4401-BC66-ED7AF20F0E43}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6595,6 +6625,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7732749D-B1A2-4E70-B7F4-898D2C27DFCA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="88b2ba63-7ebb-4a2a-9e9c-c27acabcde36"/>
+    <ds:schemaRef ds:uri="6bab19be-6345-4ed3-a392-384eca2a3a3f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4394CFF6-4A26-4CEA-BFC4-481182046E8E}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Started to implement MakeOfferPanel
</commit_message>
<xml_diff>
--- a/Localization/Texts.xlsx
+++ b/Localization/Texts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UnitySSD\VoxToVFX-2021\Localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63EEE9FC-0026-4246-A4A9-F6C47D4175C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235D7C85-6879-45F4-8DA2-4DD448C47CBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="798">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="815">
   <si>
     <t>Clé</t>
   </si>
@@ -1809,15 +1809,6 @@
     <t>[SET_BUY_AMOUNT_REQUIRED]</t>
   </si>
   <si>
-    <t>Must be at least 0.01 ETH</t>
-  </si>
-  <si>
-    <t>Doit être d'au moins 0,01 ETH</t>
-  </si>
-  <si>
-    <t>[SET_BUY_AT_LEAST_0_01ETH]</t>
-  </si>
-  <si>
     <t>Set Price</t>
   </si>
   <si>
@@ -2449,6 +2440,66 @@
   </si>
   <si>
     <t>Bought by</t>
+  </si>
+  <si>
+    <t>Make an Offer</t>
+  </si>
+  <si>
+    <t>[MAKE_OFFER_TITLE]</t>
+  </si>
+  <si>
+    <t>Once an Offer is sent, the owner will have 24 hours to accept. If the Offer expires, the funds will be available in your Marketplace Balance.</t>
+  </si>
+  <si>
+    <t>Une fois qu'une offre est envoyée, le propriétaire aura 24 heures pour accepter. Si l'offre expire, les fonds seront disponibles dans votre solde Marketplace.</t>
+  </si>
+  <si>
+    <t>[MAKE_OFFER_DESCRIPTION]</t>
+  </si>
+  <si>
+    <t>Doit être d'au moins {0} ETH</t>
+  </si>
+  <si>
+    <t>Must be at least {0} ETH</t>
+  </si>
+  <si>
+    <t>[MUST_BE_AT_LEAST_X_LABEL]</t>
+  </si>
+  <si>
+    <t>Your Offer is being confirmed on the Ethereum blockchain.</t>
+  </si>
+  <si>
+    <t>Making the Offer …</t>
+  </si>
+  <si>
+    <t>En cours d'offre …</t>
+  </si>
+  <si>
+    <t>[MAKE_OFFER_WAITING_TITLE]</t>
+  </si>
+  <si>
+    <t>[MAKE_OFFER_WAITING_DESCRIPTION]</t>
+  </si>
+  <si>
+    <t>Votre offre est en cours de confirmation sur la blockchain Ethereum.</t>
+  </si>
+  <si>
+    <t>Offer made!</t>
+  </si>
+  <si>
+    <t>Offre faite !</t>
+  </si>
+  <si>
+    <t>[MAKE_OFFER_SUCCESS_TITLE]</t>
+  </si>
+  <si>
+    <t>Your Offer has been sent to the owner. They have 24 hours to accept your offer. If not accepted, the Offer will expire and will be returned to your Marketplace Balance.</t>
+  </si>
+  <si>
+    <t>Votre offre a été envoyée au propriétaire. Il a 24 heures pour accepter votre offre. Si elle n'est pas acceptée, l'offre expirera et sera restituée à votre solde Marketplace.</t>
+  </si>
+  <si>
+    <t>[MAKE_OFFER_SUCCESS_DESCRIPTION]</t>
   </si>
 </sst>
 </file>
@@ -2904,11 +2955,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:IW274"/>
+  <dimension ref="A1:IW280"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A247" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A258" sqref="A258"/>
+      <pane ySplit="1" topLeftCell="A252" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A281" sqref="A281"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4781,10 +4832,10 @@
         <v>464</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="E158" s="2" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
@@ -4811,7 +4862,7 @@
     </row>
     <row r="161" spans="1:257" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="D161" s="2" t="s">
         <v>472</v>
@@ -5523,51 +5574,51 @@
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
-        <v>586</v>
+        <v>802</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>585</v>
+        <v>800</v>
       </c>
       <c r="E201" s="2" t="s">
-        <v>584</v>
+        <v>801</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="E202" s="2" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="D203" s="2" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="E203" s="2" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
     </row>
     <row r="204" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="E204" s="2" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="D205" s="8" t="s">
         <v>497</v>
@@ -5578,194 +5629,194 @@
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="D206" s="2" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="E206" s="2" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="D207" s="2" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="E207" s="2" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="D208" s="2" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="E208" s="2" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="E209" s="2" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="D210" s="2" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="E210" s="2" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="D211" s="2" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="E211" s="2" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="212" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="D212" s="2" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="E212" s="2" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="D213" s="2" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="E213" s="2" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="D214" s="2" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="E214" s="2" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="E215" s="2" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="D216" s="2" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="E216" s="2" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="E217" s="2" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="E218" s="2" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
     </row>
     <row r="219" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="D219" s="2" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="E219" s="2" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="D220" s="2" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="E220" s="2" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="D221" s="2" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="E221" s="2" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="D222" s="2" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="E222" s="2" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="D223" s="2" t="s">
         <v>472</v>
@@ -5776,348 +5827,348 @@
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="D224" s="2" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="E224" s="2" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="D225" s="2" t="s">
         <v>637</v>
       </c>
-      <c r="D225" s="2" t="s">
-        <v>640</v>
-      </c>
       <c r="E225" s="2" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="D226" s="2" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="E226" s="2" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
     </row>
     <row r="227" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="D227" s="2" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="E227" s="2" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="D228" s="2" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="E228" s="2" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
     </row>
     <row r="229" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="D229" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="E229" s="2" t="s">
         <v>646</v>
-      </c>
-      <c r="D229" s="2" t="s">
-        <v>648</v>
-      </c>
-      <c r="E229" s="2" t="s">
-        <v>649</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="D230" s="2" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="E230" s="2" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
     </row>
     <row r="231" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="D231" s="2" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="E231" s="2" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="D232" s="2" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="E232" s="2" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="D233" s="2" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="E233" s="2" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="D234" s="2" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="E234" s="2" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="D235" s="2" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="E235" s="2" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="D236" s="2" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
       <c r="E236" s="2" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="D237" s="2" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="E237" s="2" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="D238" s="2" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="E238" s="2" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="D239" s="2" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="E239" s="2" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="D240" s="2" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E240" s="2" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="D241" s="2" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="E241" s="2" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
     </row>
     <row r="242" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="D242" s="2" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="E242" s="2" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="D243" s="2" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="E243" s="2" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
     </row>
     <row r="244" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="D244" s="2" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="E244" s="2" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
       <c r="D245" s="2" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
       <c r="E245" s="2" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
     </row>
     <row r="246" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="D246" s="2" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="E246" s="2" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="D247" s="2" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="E247" s="2" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="D248" s="2" t="s">
         <v>723</v>
       </c>
-      <c r="D248" s="2" t="s">
-        <v>726</v>
-      </c>
       <c r="E248" s="2" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
+        <v>721</v>
+      </c>
+      <c r="D249" s="2" t="s">
         <v>724</v>
       </c>
-      <c r="D249" s="2" t="s">
-        <v>727</v>
-      </c>
       <c r="E249" s="2" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="D250" s="2" t="s">
         <v>728</v>
       </c>
-      <c r="D250" s="2" t="s">
-        <v>731</v>
-      </c>
       <c r="E250" s="2" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
     </row>
     <row r="251" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="D251" s="2" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="E251" s="2" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="D252" s="2" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="E252" s="2" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="D253" s="2" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="E253" s="2" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
       <c r="D254" s="2" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E254" s="2" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
       <c r="D255" s="2" t="s">
         <v>540</v>
@@ -6128,62 +6179,62 @@
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
       <c r="D256" s="2" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
       <c r="E256" s="2" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="D257" s="2" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="E257" s="2" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="D258" s="2" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="E258" s="2" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="D259" s="2" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="E259" s="2" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
       <c r="D260" s="2" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
       <c r="E260" s="2" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="D261" s="2" t="s">
         <v>497</v>
@@ -6194,145 +6245,211 @@
     </row>
     <row r="262" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="D262" s="2" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="E262" s="2" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="D263" s="2" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
       <c r="E263" s="2" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="D264" s="2" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="E264" s="2" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="D265" s="2" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="E265" s="2" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="D266" s="2" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="E266" s="2" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="D267" s="2" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="E267" s="2" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="D268" s="2" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="E268" s="2" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
       <c r="D269" s="2" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="E269" s="2" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
       <c r="D270" s="2" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
       <c r="E270" s="2" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="D271" s="2" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
       <c r="E271" s="2" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
       <c r="D272" s="2" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="E272" s="2" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="D273" s="2" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="E273" s="2" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="D274" s="2" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="E274" s="2" t="s">
-        <v>794</v>
+        <v>791</v>
+      </c>
+    </row>
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A275" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="D275" s="2" t="s">
+        <v>738</v>
+      </c>
+      <c r="E275" s="2" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="276" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A276" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="D276" s="2" t="s">
+        <v>798</v>
+      </c>
+      <c r="E276" s="2" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A277" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="D277" s="2" t="s">
+        <v>805</v>
+      </c>
+      <c r="E277" s="2" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A278" s="1" t="s">
+        <v>807</v>
+      </c>
+      <c r="D278" s="2" t="s">
+        <v>808</v>
+      </c>
+      <c r="E278" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A279" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="D279" s="2" t="s">
+        <v>810</v>
+      </c>
+      <c r="E279" s="2" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="280" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A280" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="D280" s="2" t="s">
+        <v>813</v>
+      </c>
+      <c r="E280" s="2" t="s">
+        <v>812</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fetch OfferMade and OfferAccepted events
</commit_message>
<xml_diff>
--- a/Localization/Texts.xlsx
+++ b/Localization/Texts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UnitySSD\VoxToVFX-2021\Localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235D7C85-6879-45F4-8DA2-4DD448C47CBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AED0CDF-573E-4028-861C-FED493CEE4C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Texts!$A$1:$IW$163</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="815">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="821">
   <si>
     <t>Clé</t>
   </si>
@@ -2298,12 +2297,6 @@
     <t>[BUY_NOW_SET_LABEL]</t>
   </si>
   <si>
-    <t>Buy Now price removed by</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prix d'achat immédiat retiré par </t>
-  </si>
-  <si>
     <t>[BUY_NOW_REMOVED_LABEL]</t>
   </si>
   <si>
@@ -2500,6 +2493,30 @@
   </si>
   <si>
     <t>[MAKE_OFFER_SUCCESS_DESCRIPTION]</t>
+  </si>
+  <si>
+    <t>[OFFER_MADE_BY_LABEL]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Offre faite par </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Offer made by </t>
+  </si>
+  <si>
+    <t>[OFFER_MADE_ACCEPTED_LABEL]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Offer accepted from </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Offre accepté de la part de </t>
+  </si>
+  <si>
+    <t>Prix d'achat immédiat retiré</t>
+  </si>
+  <si>
+    <t>Buy Now price removed</t>
   </si>
 </sst>
 </file>
@@ -2955,11 +2972,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:IW280"/>
+  <dimension ref="A1:IW282"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A252" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A281" sqref="A281"/>
+      <pane ySplit="1" topLeftCell="A242" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E260" sqref="E260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5574,13 +5591,13 @@
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="E201" s="2" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
@@ -5739,7 +5756,7 @@
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="D216" s="2" t="s">
         <v>662</v>
@@ -6190,13 +6207,13 @@
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
+        <v>790</v>
+      </c>
+      <c r="D257" s="2" t="s">
+        <v>791</v>
+      </c>
+      <c r="E257" s="2" t="s">
         <v>792</v>
-      </c>
-      <c r="D257" s="2" t="s">
-        <v>793</v>
-      </c>
-      <c r="E257" s="2" t="s">
-        <v>794</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
@@ -6212,29 +6229,29 @@
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="D259" s="2" t="s">
-        <v>748</v>
+        <v>819</v>
       </c>
       <c r="E259" s="2" t="s">
-        <v>747</v>
+        <v>820</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="D260" s="2" t="s">
+        <v>748</v>
+      </c>
+      <c r="E260" s="2" t="s">
         <v>750</v>
-      </c>
-      <c r="E260" s="2" t="s">
-        <v>752</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="D261" s="2" t="s">
         <v>497</v>
@@ -6245,211 +6262,233 @@
     </row>
     <row r="262" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="D262" s="2" t="s">
         <v>754</v>
       </c>
-      <c r="D262" s="2" t="s">
-        <v>756</v>
-      </c>
       <c r="E262" s="2" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="D263" s="2" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="E263" s="2" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="D264" s="2" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="E264" s="2" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="D265" s="2" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="E265" s="2" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="D266" s="2" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="E266" s="2" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="D267" s="2" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="E267" s="2" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="D268" s="2" t="s">
         <v>770</v>
       </c>
-      <c r="D268" s="2" t="s">
-        <v>772</v>
-      </c>
       <c r="E268" s="2" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="D269" s="2" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="E269" s="2" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="D270" s="2" t="s">
         <v>776</v>
       </c>
-      <c r="D270" s="2" t="s">
-        <v>778</v>
-      </c>
       <c r="E270" s="2" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="D271" s="2" t="s">
+        <v>782</v>
+      </c>
+      <c r="E271" s="2" t="s">
         <v>784</v>
-      </c>
-      <c r="E271" s="2" t="s">
-        <v>786</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="D272" s="2" t="s">
+        <v>783</v>
+      </c>
+      <c r="E272" s="2" t="s">
         <v>785</v>
-      </c>
-      <c r="E272" s="2" t="s">
-        <v>787</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="D273" s="2" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="E273" s="2" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
+        <v>787</v>
+      </c>
+      <c r="D274" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="E274" s="2" t="s">
         <v>789</v>
-      </c>
-      <c r="D274" s="2" t="s">
-        <v>790</v>
-      </c>
-      <c r="E274" s="2" t="s">
-        <v>791</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="D275" s="2" t="s">
         <v>738</v>
       </c>
       <c r="E275" s="2" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
     </row>
     <row r="276" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="D276" s="2" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="E276" s="2" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="D277" s="2" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="E277" s="2" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="D278" s="2" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="E278" s="2" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="D279" s="2" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="E279" s="2" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
     </row>
     <row r="280" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="D280" s="2" t="s">
+        <v>811</v>
+      </c>
+      <c r="E280" s="2" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A281" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="D281" s="2" t="s">
         <v>814</v>
       </c>
-      <c r="D280" s="2" t="s">
-        <v>813</v>
-      </c>
-      <c r="E280" s="2" t="s">
-        <v>812</v>
+      <c r="E281" s="2" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A282" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="D282" s="2" t="s">
+        <v>818</v>
+      </c>
+      <c r="E282" s="2" t="s">
+        <v>817</v>
       </c>
     </row>
   </sheetData>

</xml_diff>